<commit_message>
SIF 2 Facturacion Terminado, Revisar numeros y corregir
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/comprobantes a desestimar.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/comprobantes a desestimar.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Desktop\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iachenbach\Gobierno de la Ciudad de Buenos Aires\Pablo Alfredo Gadea - Tablero Facoep P BI\FACOEP\DBA\Reportes BI\2021\Facturación\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +373,7 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>